<commit_message>
* updated categories * added previously missing programs to category plots * fixed wrong correlation in some estimates files * many small fixes
</commit_message>
<xml_diff>
--- a/estimates/OneEuroJobs.xlsx
+++ b/estimates/OneEuroJobs.xlsx
@@ -961,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A14:L25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J14:J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,7 +1313,7 @@
         <v>0.01</v>
       </c>
       <c r="J14">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>39</v>
@@ -1336,7 +1336,7 @@
         <v>0.01</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>39</v>
@@ -1359,7 +1359,7 @@
         <v>0.01</v>
       </c>
       <c r="J16">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>39</v>
@@ -1382,7 +1382,7 @@
         <v>0.01</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>39</v>
@@ -1405,7 +1405,7 @@
         <v>0.01</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>39</v>
@@ -1428,7 +1428,7 @@
         <v>0.01</v>
       </c>
       <c r="J19">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>39</v>
@@ -1451,7 +1451,7 @@
         <v>0.01</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>39</v>
@@ -1474,7 +1474,7 @@
         <v>0.01</v>
       </c>
       <c r="J21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>39</v>
@@ -1497,7 +1497,7 @@
         <v>0.01</v>
       </c>
       <c r="J22">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>39</v>
@@ -1520,7 +1520,7 @@
         <v>0.01</v>
       </c>
       <c r="J23">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>39</v>
@@ -1543,7 +1543,7 @@
         <v>0.01</v>
       </c>
       <c r="J24">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>39</v>
@@ -1566,7 +1566,7 @@
         <v>0.01</v>
       </c>
       <c r="J25">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
* also update excel files
</commit_message>
<xml_diff>
--- a/estimates/OneEuroJobs.xlsx
+++ b/estimates/OneEuroJobs.xlsx
@@ -63,42 +63,6 @@
     <t>https://ideas.repec.org/p/iab/iabdpa/201021.html</t>
   </si>
   <si>
-    <t>monthly_gross_earnings_effect_female_east_year1</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_female_west_year1</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_male_west_year1</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_male_east_year1</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_female_west_year2</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_female_east_year2</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_male_west_year2</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_male_east_year2</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_female_west_year3</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_female_east_year3</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_male_west_year3</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_male_east_year3</t>
-  </si>
-  <si>
     <t>Hohmeyer &amp; Wolff (2010), Table 13</t>
   </si>
   <si>
@@ -139,6 +103,42 @@
   </si>
   <si>
     <t>Hohmeyer &amp; Wolff (2010), Table 15</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_female_west_year1</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_female_east_year1</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_male_west_year1</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_male_east_year1</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_female_west_year2</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_female_east_year2</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_male_west_year2</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_male_east_year2</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_female_west_year3</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_female_east_year3</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_male_west_year3</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_male_east_year3</t>
   </si>
 </sst>
 </file>
@@ -962,7 +962,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J14:J25"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,7 +1025,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>-181</v>
@@ -1040,7 +1040,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>13</v>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>-230</v>
@@ -1063,7 +1063,7 @@
         <v>1</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>13</v>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>-281</v>
@@ -1086,7 +1086,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>13</v>
@@ -1094,7 +1094,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>-414</v>
@@ -1109,7 +1109,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>13</v>
@@ -1117,7 +1117,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>183</v>
@@ -1132,7 +1132,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>13</v>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B7">
         <v>-72</v>
@@ -1155,7 +1155,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>13</v>
@@ -1163,7 +1163,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B8">
         <v>-1</v>
@@ -1178,7 +1178,7 @@
         <v>1</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>13</v>
@@ -1186,7 +1186,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B9">
         <v>-382</v>
@@ -1201,7 +1201,7 @@
         <v>1</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>13</v>
@@ -1209,7 +1209,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B10">
         <v>357</v>
@@ -1224,7 +1224,7 @@
         <v>1</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>13</v>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B11">
         <v>137</v>
@@ -1247,7 +1247,7 @@
         <v>1</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>13</v>
@@ -1255,7 +1255,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B12">
         <v>117</v>
@@ -1270,7 +1270,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>13</v>
@@ -1278,7 +1278,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B13">
         <v>-176</v>
@@ -1293,7 +1293,7 @@
         <v>1</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>13</v>
@@ -1301,7 +1301,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>35</v>
@@ -1316,7 +1316,7 @@
         <v>-1</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>13</v>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>27</v>
@@ -1339,7 +1339,7 @@
         <v>-1</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>13</v>
@@ -1347,7 +1347,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>32</v>
@@ -1362,7 +1362,7 @@
         <v>-1</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>13</v>
@@ -1370,7 +1370,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>31</v>
@@ -1385,7 +1385,7 @@
         <v>-1</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>13</v>
@@ -1393,7 +1393,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>22</v>
@@ -1408,7 +1408,7 @@
         <v>-1</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>13</v>
@@ -1416,7 +1416,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>14</v>
@@ -1431,7 +1431,7 @@
         <v>-1</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>13</v>
@@ -1439,7 +1439,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -1454,7 +1454,7 @@
         <v>-1</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>13</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>15</v>
@@ -1477,7 +1477,7 @@
         <v>-1</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>13</v>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B22">
         <v>19</v>
@@ -1500,7 +1500,7 @@
         <v>-1</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>13</v>
@@ -1508,7 +1508,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>11</v>
@@ -1523,7 +1523,7 @@
         <v>-1</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>13</v>
@@ -1531,7 +1531,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B24">
         <v>16</v>
@@ -1546,7 +1546,7 @@
         <v>-1</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>13</v>
@@ -1554,7 +1554,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>12</v>
@@ -1569,7 +1569,7 @@
         <v>-1</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>13</v>

</xml_diff>